<commit_message>
I have updated  the sort order to display questions and jump in navigation and download for NRG also.
</commit_message>
<xml_diff>
--- a/Project_Files/Testing/meta.xlsx
+++ b/Project_Files/Testing/meta.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internal\Tabulation\Project_Files\MR\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Internal\Tabulation\Project_Files\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7ACC9085-9F56-40EC-AE9F-2C5F7DB2ED06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6073806D-459E-43AC-8EBC-E5CEB419FE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,9 @@
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
     <sheet name="value_label" sheetId="2" r:id="rId2"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId3"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1856" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1857" uniqueCount="438">
   <si>
     <t>Var_Name</t>
   </si>
@@ -1342,6 +1345,12 @@
   </si>
   <si>
     <t>Numeric grid</t>
+  </si>
+  <si>
+    <t>Sortorder</t>
+  </si>
+  <si>
+    <t>Date</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1387,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1401,16 +1410,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1428,6 +1451,204 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>E31</v>
+          </cell>
+          <cell r="B1">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="2">
+          <cell r="A2" t="str">
+            <v>E11</v>
+          </cell>
+          <cell r="B2">
+            <v>2</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>E10</v>
+          </cell>
+          <cell r="B3">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>E8</v>
+          </cell>
+          <cell r="B4">
+            <v>4</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Q4</v>
+          </cell>
+          <cell r="B5">
+            <v>5</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>E17</v>
+          </cell>
+          <cell r="B6">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>E12</v>
+          </cell>
+          <cell r="B7">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>E14</v>
+          </cell>
+          <cell r="B8">
+            <v>8</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>E13</v>
+          </cell>
+          <cell r="B9">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>E22</v>
+          </cell>
+          <cell r="B10">
+            <v>10</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>E26</v>
+          </cell>
+          <cell r="B11">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>E23</v>
+          </cell>
+          <cell r="B12">
+            <v>12</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>E27</v>
+          </cell>
+          <cell r="B13">
+            <v>13</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>E24</v>
+          </cell>
+          <cell r="B14">
+            <v>14</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="A15" t="str">
+            <v>E28</v>
+          </cell>
+          <cell r="B15">
+            <v>15</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>E6</v>
+          </cell>
+          <cell r="B16">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>E25</v>
+          </cell>
+          <cell r="B17">
+            <v>17</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>E29</v>
+          </cell>
+          <cell r="B18">
+            <v>18</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>E30</v>
+          </cell>
+          <cell r="B19">
+            <v>19</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>FI_E10</v>
+          </cell>
+          <cell r="B20">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>FI_E12</v>
+          </cell>
+          <cell r="B21">
+            <v>21</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>FL_E10</v>
+          </cell>
+          <cell r="B22">
+            <v>22</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>FL_E12</v>
+          </cell>
+          <cell r="B23">
+            <v>23</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1715,10 +1936,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H169"/>
+  <dimension ref="A1:I169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1733,7 +1954,7 @@
     <col min="8" max="8" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1758,8 +1979,11 @@
       <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1770,7 +1994,7 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>343</v>
+        <v>437</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -1778,8 +2002,12 @@
       <c r="F2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2">
+        <f>VLOOKUP(E2,[1]Sheet1!$A:$B,2,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1798,8 +2026,12 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <f>VLOOKUP(E3,[1]Sheet1!$A:$B,2,0)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -1818,8 +2050,12 @@
       <c r="F4" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <f>VLOOKUP(E4,[1]Sheet1!$A:$B,2,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1838,8 +2074,12 @@
       <c r="F5" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <f>VLOOKUP(E5,[1]Sheet1!$A:$B,2,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -1858,8 +2098,12 @@
       <c r="F6" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <f>VLOOKUP(E6,[1]Sheet1!$A:$B,2,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1878,8 +2122,12 @@
       <c r="F7" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <f>VLOOKUP(E7,[1]Sheet1!$A:$B,2,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1898,8 +2146,12 @@
       <c r="F8" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <f>VLOOKUP(E8,[1]Sheet1!$A:$B,2,0)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1918,8 +2170,12 @@
       <c r="F9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <f>VLOOKUP(E9,[1]Sheet1!$A:$B,2,0)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1938,8 +2194,12 @@
       <c r="F10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <f>VLOOKUP(E10,[1]Sheet1!$A:$B,2,0)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -1961,8 +2221,12 @@
       <c r="H11" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <f>VLOOKUP(E11,[1]Sheet1!$A:$B,2,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1984,8 +2248,12 @@
       <c r="H12" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <f>VLOOKUP(E12,[1]Sheet1!$A:$B,2,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -2007,8 +2275,12 @@
       <c r="H13" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <f>VLOOKUP(E13,[1]Sheet1!$A:$B,2,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -2030,8 +2302,12 @@
       <c r="H14" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f>VLOOKUP(E14,[1]Sheet1!$A:$B,2,0)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>25</v>
       </c>
@@ -2050,8 +2326,12 @@
       <c r="F15" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <f>VLOOKUP(E15,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -2070,8 +2350,12 @@
       <c r="F16" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <f>VLOOKUP(E16,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -2090,8 +2374,12 @@
       <c r="F17" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <f>VLOOKUP(E17,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -2110,8 +2398,12 @@
       <c r="F18" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <f>VLOOKUP(E18,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>29</v>
       </c>
@@ -2130,8 +2422,12 @@
       <c r="F19" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <f>VLOOKUP(E19,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>30</v>
       </c>
@@ -2150,8 +2446,12 @@
       <c r="F20" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <f>VLOOKUP(E20,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -2170,8 +2470,12 @@
       <c r="F21" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <f>VLOOKUP(E21,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2190,8 +2494,12 @@
       <c r="F22" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <f>VLOOKUP(E22,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>33</v>
       </c>
@@ -2210,8 +2518,12 @@
       <c r="F23" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <f>VLOOKUP(E23,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2230,8 +2542,12 @@
       <c r="F24" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <f>VLOOKUP(E24,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2250,8 +2566,12 @@
       <c r="F25" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <f>VLOOKUP(E25,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>36</v>
       </c>
@@ -2270,8 +2590,12 @@
       <c r="F26" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <f>VLOOKUP(E26,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>37</v>
       </c>
@@ -2290,8 +2614,12 @@
       <c r="F27" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <f>VLOOKUP(E27,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>38</v>
       </c>
@@ -2310,8 +2638,12 @@
       <c r="F28" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <f>VLOOKUP(E28,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>39</v>
       </c>
@@ -2330,8 +2662,12 @@
       <c r="F29" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <f>VLOOKUP(E29,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>40</v>
       </c>
@@ -2350,8 +2686,12 @@
       <c r="F30" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <f>VLOOKUP(E30,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -2370,8 +2710,12 @@
       <c r="F31" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <f>VLOOKUP(E31,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>42</v>
       </c>
@@ -2390,8 +2734,12 @@
       <c r="F32" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <f>VLOOKUP(E32,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>43</v>
       </c>
@@ -2410,8 +2758,12 @@
       <c r="F33" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <f>VLOOKUP(E33,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>44</v>
       </c>
@@ -2430,8 +2782,12 @@
       <c r="F34" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <f>VLOOKUP(E34,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>45</v>
       </c>
@@ -2450,8 +2806,12 @@
       <c r="F35" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <f>VLOOKUP(E35,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -2470,8 +2830,12 @@
       <c r="F36" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <f>VLOOKUP(E36,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -2490,8 +2854,12 @@
       <c r="F37" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <f>VLOOKUP(E37,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>48</v>
       </c>
@@ -2510,8 +2878,12 @@
       <c r="F38" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <f>VLOOKUP(E38,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>49</v>
       </c>
@@ -2530,8 +2902,12 @@
       <c r="F39" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <f>VLOOKUP(E39,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>50</v>
       </c>
@@ -2550,8 +2926,12 @@
       <c r="F40" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <f>VLOOKUP(E40,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>51</v>
       </c>
@@ -2570,8 +2950,12 @@
       <c r="F41" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <f>VLOOKUP(E41,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>52</v>
       </c>
@@ -2590,8 +2974,12 @@
       <c r="F42" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <f>VLOOKUP(E42,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>53</v>
       </c>
@@ -2610,8 +2998,12 @@
       <c r="F43" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <f>VLOOKUP(E43,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>54</v>
       </c>
@@ -2630,8 +3022,12 @@
       <c r="F44" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <f>VLOOKUP(E44,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -2650,8 +3046,12 @@
       <c r="F45" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <f>VLOOKUP(E45,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>56</v>
       </c>
@@ -2670,8 +3070,12 @@
       <c r="F46" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <f>VLOOKUP(E46,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>57</v>
       </c>
@@ -2690,8 +3094,12 @@
       <c r="F47" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <f>VLOOKUP(E47,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -2710,8 +3118,12 @@
       <c r="F48" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <f>VLOOKUP(E48,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>59</v>
       </c>
@@ -2730,8 +3142,12 @@
       <c r="F49" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <f>VLOOKUP(E49,[1]Sheet1!$A:$B,2,0)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -2750,8 +3166,12 @@
       <c r="F50" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <f>VLOOKUP(E50,[1]Sheet1!$A:$B,2,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>62</v>
       </c>
@@ -2770,8 +3190,12 @@
       <c r="F51" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <f>VLOOKUP(E51,[1]Sheet1!$A:$B,2,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>64</v>
       </c>
@@ -2790,8 +3214,12 @@
       <c r="F52" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <f>VLOOKUP(E52,[1]Sheet1!$A:$B,2,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>66</v>
       </c>
@@ -2810,8 +3238,12 @@
       <c r="F53" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <f>VLOOKUP(E53,[1]Sheet1!$A:$B,2,0)</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>68</v>
       </c>
@@ -2830,8 +3262,12 @@
       <c r="F54" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <f>VLOOKUP(E54,[1]Sheet1!$A:$B,2,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>69</v>
       </c>
@@ -2850,8 +3286,12 @@
       <c r="F55" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <f>VLOOKUP(E55,[1]Sheet1!$A:$B,2,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>70</v>
       </c>
@@ -2870,8 +3310,12 @@
       <c r="F56" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <f>VLOOKUP(E56,[1]Sheet1!$A:$B,2,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>71</v>
       </c>
@@ -2890,8 +3334,12 @@
       <c r="F57" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <f>VLOOKUP(E57,[1]Sheet1!$A:$B,2,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>72</v>
       </c>
@@ -2910,8 +3358,12 @@
       <c r="F58" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58">
+        <f>VLOOKUP(E58,[1]Sheet1!$A:$B,2,0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>73</v>
       </c>
@@ -2933,8 +3385,12 @@
       <c r="H59" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59">
+        <f>VLOOKUP(E59,[1]Sheet1!$A:$B,2,0)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>75</v>
       </c>
@@ -2956,8 +3412,12 @@
       <c r="H60" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <f>VLOOKUP(E60,[1]Sheet1!$A:$B,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>77</v>
       </c>
@@ -2979,8 +3439,12 @@
       <c r="H61" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <f>VLOOKUP(E61,[1]Sheet1!$A:$B,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>79</v>
       </c>
@@ -3002,8 +3466,12 @@
       <c r="H62" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <f>VLOOKUP(E62,[1]Sheet1!$A:$B,2,0)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>81</v>
       </c>
@@ -3025,8 +3493,12 @@
       <c r="H63" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <f>VLOOKUP(E63,[1]Sheet1!$A:$B,2,0)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -3048,8 +3520,12 @@
       <c r="H64" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <f>VLOOKUP(E64,[1]Sheet1!$A:$B,2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>85</v>
       </c>
@@ -3071,8 +3547,12 @@
       <c r="H65" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <f>VLOOKUP(E65,[1]Sheet1!$A:$B,2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>87</v>
       </c>
@@ -3094,8 +3574,12 @@
       <c r="H66" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <f>VLOOKUP(E66,[1]Sheet1!$A:$B,2,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>89</v>
       </c>
@@ -3117,8 +3601,12 @@
       <c r="H67" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <f>VLOOKUP(E67,[1]Sheet1!$A:$B,2,0)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>91</v>
       </c>
@@ -3140,8 +3628,12 @@
       <c r="H68" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <f>VLOOKUP(E68,[1]Sheet1!$A:$B,2,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>93</v>
       </c>
@@ -3163,8 +3655,12 @@
       <c r="H69" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <f>VLOOKUP(E69,[1]Sheet1!$A:$B,2,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>95</v>
       </c>
@@ -3186,8 +3682,12 @@
       <c r="H70" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70">
+        <f>VLOOKUP(E70,[1]Sheet1!$A:$B,2,0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>97</v>
       </c>
@@ -3209,8 +3709,12 @@
       <c r="H71" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71">
+        <f>VLOOKUP(E71,[1]Sheet1!$A:$B,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>99</v>
       </c>
@@ -3232,8 +3736,12 @@
       <c r="H72" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72">
+        <f>VLOOKUP(E72,[1]Sheet1!$A:$B,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>101</v>
       </c>
@@ -3255,8 +3763,12 @@
       <c r="H73" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73">
+        <f>VLOOKUP(E73,[1]Sheet1!$A:$B,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>103</v>
       </c>
@@ -3278,8 +3790,12 @@
       <c r="H74" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74">
+        <f>VLOOKUP(E74,[1]Sheet1!$A:$B,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>105</v>
       </c>
@@ -3301,8 +3817,12 @@
       <c r="H75" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75">
+        <f>VLOOKUP(E75,[1]Sheet1!$A:$B,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>107</v>
       </c>
@@ -3324,8 +3844,12 @@
       <c r="H76" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76">
+        <f>VLOOKUP(E76,[1]Sheet1!$A:$B,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>109</v>
       </c>
@@ -3347,8 +3871,12 @@
       <c r="H77" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77">
+        <f>VLOOKUP(E77,[1]Sheet1!$A:$B,2,0)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>111</v>
       </c>
@@ -3367,8 +3895,12 @@
       <c r="F78" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78">
+        <f>VLOOKUP(E78,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>113</v>
       </c>
@@ -3387,8 +3919,12 @@
       <c r="F79" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79">
+        <f>VLOOKUP(E79,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>115</v>
       </c>
@@ -3407,8 +3943,12 @@
       <c r="F80" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80">
+        <f>VLOOKUP(E80,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>117</v>
       </c>
@@ -3427,8 +3967,12 @@
       <c r="F81" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81">
+        <f>VLOOKUP(E81,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>119</v>
       </c>
@@ -3447,8 +3991,12 @@
       <c r="F82" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82">
+        <f>VLOOKUP(E82,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>121</v>
       </c>
@@ -3467,8 +4015,12 @@
       <c r="F83" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83">
+        <f>VLOOKUP(E83,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>123</v>
       </c>
@@ -3487,8 +4039,12 @@
       <c r="F84" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84">
+        <f>VLOOKUP(E84,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>125</v>
       </c>
@@ -3507,8 +4063,12 @@
       <c r="F85" t="s">
         <v>405</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85">
+        <f>VLOOKUP(E85,[1]Sheet1!$A:$B,2,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>127</v>
       </c>
@@ -3530,8 +4090,12 @@
       <c r="H86" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86">
+        <f>VLOOKUP(E86,[1]Sheet1!$A:$B,2,0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>129</v>
       </c>
@@ -3553,8 +4117,12 @@
       <c r="H87" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87">
+        <f>VLOOKUP(E87,[1]Sheet1!$A:$B,2,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>131</v>
       </c>
@@ -3576,8 +4144,12 @@
       <c r="H88" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88">
+        <f>VLOOKUP(E88,[1]Sheet1!$A:$B,2,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>133</v>
       </c>
@@ -3599,8 +4171,12 @@
       <c r="H89" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89">
+        <f>VLOOKUP(E89,[1]Sheet1!$A:$B,2,0)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>141</v>
       </c>
@@ -3619,8 +4195,12 @@
       <c r="F90" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90">
+        <f>VLOOKUP(E90,[1]Sheet1!$A:$B,2,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>143</v>
       </c>
@@ -3639,8 +4219,12 @@
       <c r="F91" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91">
+        <f>VLOOKUP(E91,[1]Sheet1!$A:$B,2,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>145</v>
       </c>
@@ -3659,8 +4243,12 @@
       <c r="F92" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92">
+        <f>VLOOKUP(E92,[1]Sheet1!$A:$B,2,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>147</v>
       </c>
@@ -3679,8 +4267,12 @@
       <c r="F93" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93">
+        <f>VLOOKUP(E93,[1]Sheet1!$A:$B,2,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>149</v>
       </c>
@@ -3699,8 +4291,12 @@
       <c r="F94" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94">
+        <f>VLOOKUP(E94,[1]Sheet1!$A:$B,2,0)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>151</v>
       </c>
@@ -3719,8 +4315,12 @@
       <c r="F95" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95">
+        <f>VLOOKUP(E95,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>152</v>
       </c>
@@ -3739,8 +4339,12 @@
       <c r="F96" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I96">
+        <f>VLOOKUP(E96,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>153</v>
       </c>
@@ -3759,8 +4363,12 @@
       <c r="F97" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I97">
+        <f>VLOOKUP(E97,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>154</v>
       </c>
@@ -3779,8 +4387,12 @@
       <c r="F98" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I98">
+        <f>VLOOKUP(E98,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>155</v>
       </c>
@@ -3799,8 +4411,12 @@
       <c r="F99" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I99">
+        <f>VLOOKUP(E99,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>156</v>
       </c>
@@ -3819,8 +4435,12 @@
       <c r="F100" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I100">
+        <f>VLOOKUP(E100,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>157</v>
       </c>
@@ -3839,8 +4459,12 @@
       <c r="F101" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I101">
+        <f>VLOOKUP(E101,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>158</v>
       </c>
@@ -3859,8 +4483,12 @@
       <c r="F102" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I102">
+        <f>VLOOKUP(E102,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>159</v>
       </c>
@@ -3879,8 +4507,12 @@
       <c r="F103" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I103">
+        <f>VLOOKUP(E103,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>160</v>
       </c>
@@ -3899,8 +4531,12 @@
       <c r="F104" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I104">
+        <f>VLOOKUP(E104,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>161</v>
       </c>
@@ -3919,8 +4555,12 @@
       <c r="F105" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I105">
+        <f>VLOOKUP(E105,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>162</v>
       </c>
@@ -3939,8 +4579,12 @@
       <c r="F106" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I106">
+        <f>VLOOKUP(E106,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>163</v>
       </c>
@@ -3959,8 +4603,12 @@
       <c r="F107" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I107">
+        <f>VLOOKUP(E107,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>164</v>
       </c>
@@ -3979,8 +4627,12 @@
       <c r="F108" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I108">
+        <f>VLOOKUP(E108,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>165</v>
       </c>
@@ -3999,8 +4651,12 @@
       <c r="F109" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I109">
+        <f>VLOOKUP(E109,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>166</v>
       </c>
@@ -4019,8 +4675,12 @@
       <c r="F110" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I110">
+        <f>VLOOKUP(E110,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>167</v>
       </c>
@@ -4039,8 +4699,12 @@
       <c r="F111" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I111">
+        <f>VLOOKUP(E111,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>168</v>
       </c>
@@ -4059,8 +4723,12 @@
       <c r="F112" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I112">
+        <f>VLOOKUP(E112,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>169</v>
       </c>
@@ -4079,8 +4747,12 @@
       <c r="F113" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I113">
+        <f>VLOOKUP(E113,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>170</v>
       </c>
@@ -4099,8 +4771,12 @@
       <c r="F114" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I114">
+        <f>VLOOKUP(E114,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>171</v>
       </c>
@@ -4119,8 +4795,12 @@
       <c r="F115" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I115">
+        <f>VLOOKUP(E115,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>172</v>
       </c>
@@ -4139,8 +4819,12 @@
       <c r="F116" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I116">
+        <f>VLOOKUP(E116,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>173</v>
       </c>
@@ -4159,8 +4843,12 @@
       <c r="F117" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I117">
+        <f>VLOOKUP(E117,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>174</v>
       </c>
@@ -4179,8 +4867,12 @@
       <c r="F118" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I118">
+        <f>VLOOKUP(E118,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>175</v>
       </c>
@@ -4199,8 +4891,12 @@
       <c r="F119" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I119">
+        <f>VLOOKUP(E119,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>176</v>
       </c>
@@ -4219,8 +4915,12 @@
       <c r="F120" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I120">
+        <f>VLOOKUP(E120,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>177</v>
       </c>
@@ -4239,8 +4939,12 @@
       <c r="F121" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I121">
+        <f>VLOOKUP(E121,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>178</v>
       </c>
@@ -4259,8 +4963,12 @@
       <c r="F122" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I122">
+        <f>VLOOKUP(E122,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>179</v>
       </c>
@@ -4279,8 +4987,12 @@
       <c r="F123" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I123">
+        <f>VLOOKUP(E123,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>180</v>
       </c>
@@ -4299,8 +5011,12 @@
       <c r="F124" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I124">
+        <f>VLOOKUP(E124,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>181</v>
       </c>
@@ -4319,8 +5035,12 @@
       <c r="F125" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I125">
+        <f>VLOOKUP(E125,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>182</v>
       </c>
@@ -4339,8 +5059,12 @@
       <c r="F126" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I126">
+        <f>VLOOKUP(E126,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>183</v>
       </c>
@@ -4359,8 +5083,12 @@
       <c r="F127" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I127">
+        <f>VLOOKUP(E127,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>184</v>
       </c>
@@ -4379,8 +5107,12 @@
       <c r="F128" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I128">
+        <f>VLOOKUP(E128,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>185</v>
       </c>
@@ -4399,8 +5131,12 @@
       <c r="F129" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I129">
+        <f>VLOOKUP(E129,[1]Sheet1!$A:$B,2,0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>337</v>
       </c>
@@ -4419,8 +5155,12 @@
       <c r="F130" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I130">
+        <f>VLOOKUP(E130,[1]Sheet1!$A:$B,2,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>338</v>
       </c>
@@ -4439,8 +5179,12 @@
       <c r="F131" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I131">
+        <f>VLOOKUP(E131,[1]Sheet1!$A:$B,2,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>339</v>
       </c>
@@ -4459,8 +5203,12 @@
       <c r="F132" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I132">
+        <f>VLOOKUP(E132,[1]Sheet1!$A:$B,2,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>340</v>
       </c>
@@ -4479,8 +5227,12 @@
       <c r="F133" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I133">
+        <f>VLOOKUP(E133,[1]Sheet1!$A:$B,2,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>341</v>
       </c>
@@ -4499,8 +5251,12 @@
       <c r="F134" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I134">
+        <f>VLOOKUP(E134,[1]Sheet1!$A:$B,2,0)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>186</v>
       </c>
@@ -4519,8 +5275,12 @@
       <c r="F135" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I135">
+        <f>VLOOKUP(E135,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>187</v>
       </c>
@@ -4539,8 +5299,12 @@
       <c r="F136" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I136">
+        <f>VLOOKUP(E136,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>188</v>
       </c>
@@ -4559,8 +5323,12 @@
       <c r="F137" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I137">
+        <f>VLOOKUP(E137,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>189</v>
       </c>
@@ -4579,8 +5347,12 @@
       <c r="F138" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I138">
+        <f>VLOOKUP(E138,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>190</v>
       </c>
@@ -4599,8 +5371,12 @@
       <c r="F139" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I139">
+        <f>VLOOKUP(E139,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>191</v>
       </c>
@@ -4619,8 +5395,12 @@
       <c r="F140" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I140">
+        <f>VLOOKUP(E140,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>192</v>
       </c>
@@ -4639,8 +5419,12 @@
       <c r="F141" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I141">
+        <f>VLOOKUP(E141,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>193</v>
       </c>
@@ -4659,8 +5443,12 @@
       <c r="F142" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I142">
+        <f>VLOOKUP(E142,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>194</v>
       </c>
@@ -4679,8 +5467,12 @@
       <c r="F143" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I143">
+        <f>VLOOKUP(E143,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>195</v>
       </c>
@@ -4699,8 +5491,12 @@
       <c r="F144" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I144">
+        <f>VLOOKUP(E144,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>196</v>
       </c>
@@ -4719,8 +5515,12 @@
       <c r="F145" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I145">
+        <f>VLOOKUP(E145,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>197</v>
       </c>
@@ -4739,8 +5539,12 @@
       <c r="F146" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I146">
+        <f>VLOOKUP(E146,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>198</v>
       </c>
@@ -4759,8 +5563,12 @@
       <c r="F147" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I147">
+        <f>VLOOKUP(E147,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>199</v>
       </c>
@@ -4779,8 +5587,12 @@
       <c r="F148" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I148">
+        <f>VLOOKUP(E148,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>200</v>
       </c>
@@ -4799,8 +5611,12 @@
       <c r="F149" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I149">
+        <f>VLOOKUP(E149,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>201</v>
       </c>
@@ -4819,8 +5635,12 @@
       <c r="F150" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I150">
+        <f>VLOOKUP(E150,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>202</v>
       </c>
@@ -4839,8 +5659,12 @@
       <c r="F151" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I151">
+        <f>VLOOKUP(E151,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>203</v>
       </c>
@@ -4859,8 +5683,12 @@
       <c r="F152" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I152">
+        <f>VLOOKUP(E152,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>204</v>
       </c>
@@ -4879,8 +5707,12 @@
       <c r="F153" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I153">
+        <f>VLOOKUP(E153,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>205</v>
       </c>
@@ -4899,8 +5731,12 @@
       <c r="F154" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I154">
+        <f>VLOOKUP(E154,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>206</v>
       </c>
@@ -4919,8 +5755,12 @@
       <c r="F155" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I155">
+        <f>VLOOKUP(E155,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>207</v>
       </c>
@@ -4939,8 +5779,12 @@
       <c r="F156" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I156">
+        <f>VLOOKUP(E156,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>208</v>
       </c>
@@ -4959,8 +5803,12 @@
       <c r="F157" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I157">
+        <f>VLOOKUP(E157,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>209</v>
       </c>
@@ -4979,8 +5827,12 @@
       <c r="F158" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I158">
+        <f>VLOOKUP(E158,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>210</v>
       </c>
@@ -4999,8 +5851,12 @@
       <c r="F159" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I159">
+        <f>VLOOKUP(E159,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>211</v>
       </c>
@@ -5019,8 +5875,12 @@
       <c r="F160" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I160">
+        <f>VLOOKUP(E160,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>212</v>
       </c>
@@ -5039,8 +5899,12 @@
       <c r="F161" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I161">
+        <f>VLOOKUP(E161,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>213</v>
       </c>
@@ -5059,8 +5923,12 @@
       <c r="F162" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I162">
+        <f>VLOOKUP(E162,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>214</v>
       </c>
@@ -5079,8 +5947,12 @@
       <c r="F163" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I163">
+        <f>VLOOKUP(E163,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>215</v>
       </c>
@@ -5099,8 +5971,12 @@
       <c r="F164" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I164">
+        <f>VLOOKUP(E164,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>216</v>
       </c>
@@ -5119,8 +5995,12 @@
       <c r="F165" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I165">
+        <f>VLOOKUP(E165,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>217</v>
       </c>
@@ -5139,8 +6019,12 @@
       <c r="F166" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I166">
+        <f>VLOOKUP(E166,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>218</v>
       </c>
@@ -5159,8 +6043,12 @@
       <c r="F167" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I167">
+        <f>VLOOKUP(E167,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>219</v>
       </c>
@@ -5179,8 +6067,12 @@
       <c r="F168" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I168">
+        <f>VLOOKUP(E168,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>220</v>
       </c>
@@ -5199,9 +6091,14 @@
       <c r="F169" t="s">
         <v>434</v>
       </c>
+      <c r="I169">
+        <f>VLOOKUP(E169,[1]Sheet1!$A:$B,2,0)</f>
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>